<commit_message>
Add opportunity to add info to existing table
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -444,222 +444,202 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Левадский</t>
+          <t>Катамахин</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Григорий</t>
+          <t>Пётр</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Яковлевич</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Лазурский</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Аркадий</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Виталиевич</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Вислоушкин</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Семён</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Данилович</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Голдякова</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ксения</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Леонидовна</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Корбуков</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Степан</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>Борисович</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Томарина</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Вероника</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Аркадьевна</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Габаев</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Валерий</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Олегович</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Серавина</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Ольга</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Федоровна</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Салибеков</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Григорий</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Яковлевич</t>
-        </is>
-      </c>
-    </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Москинов</t>
+          <t>Шабуцкий</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Виктор</t>
+          <t>Виталий</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Олегович</t>
+          <t>Юрьевич</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Варзин</t>
+          <t>Морская</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Леонид</t>
+          <t>Лариса</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Юриевич</t>
+          <t>Игоревна</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ширев</t>
+          <t>Лупков</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Илья</t>
+          <t>Анатолий</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Данилович</t>
+          <t>Леонидович</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Мигаева</t>
+          <t>Зютина</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Алёна</t>
+          <t>Дарья</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Аркадьевна</t>
+          <t>Леонидовна</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="A11" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Дурицкая</t>
+          <t>Зеверов</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Раиса</t>
+          <t>Артём</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Викторовна</t>
+          <t>Виталиевич</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add opportunity to choose create a new table or add info to existing file
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -449,17 +449,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Катамахин</t>
+          <t>Автонеева</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Пётр</t>
+          <t>Катерина</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Яковлевич</t>
+          <t>Николаевна</t>
         </is>
       </c>
     </row>
@@ -469,17 +469,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Лазурский</t>
+          <t>Щиборин</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Аркадий</t>
+          <t>Владимир</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Виталиевич</t>
+          <t>Георгиевич</t>
         </is>
       </c>
     </row>
@@ -489,17 +489,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Вислоушкин</t>
+          <t>Сивриков</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Семён</t>
+          <t>Дмитрий</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Данилович</t>
+          <t>Петрович</t>
         </is>
       </c>
     </row>
@@ -509,17 +509,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Голдякова</t>
+          <t>Позов</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ксения</t>
+          <t>Леонид</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Леонидовна</t>
+          <t>Николаевич</t>
         </is>
       </c>
     </row>
@@ -529,17 +529,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Корбуков</t>
+          <t>Сымшикова</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Степан</t>
+          <t>Алла</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Борисович</t>
+          <t>Василевна</t>
         </is>
       </c>
     </row>
@@ -549,17 +549,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Шабуцкий</t>
+          <t>Шогина</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Виталий</t>
+          <t>Полина</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Юрьевич</t>
+          <t>Евгеньевна</t>
         </is>
       </c>
     </row>
@@ -569,17 +569,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Морская</t>
+          <t>Налютин</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Лариса</t>
+          <t>Олег</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Игоревна</t>
+          <t>Евгеньевич</t>
         </is>
       </c>
     </row>
@@ -589,17 +589,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Лупков</t>
+          <t>Буртынкин</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Анатолий</t>
+          <t>Вячеслав</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Леонидович</t>
+          <t>Петрович</t>
         </is>
       </c>
     </row>
@@ -609,17 +609,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Зютина</t>
+          <t>Пикарова</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Дарья</t>
+          <t>Ольга</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Леонидовна</t>
+          <t>Олеговна</t>
         </is>
       </c>
     </row>
@@ -629,17 +629,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Зеверов</t>
+          <t>Годовкин</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Артём</t>
+          <t>Илья</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Виталиевич</t>
+          <t>Юриевич</t>
         </is>
       </c>
     </row>

</xml_diff>